<commit_message>
updated notes with ATP
</commit_message>
<xml_diff>
--- a/SAP/Notes/Notes.xlsx
+++ b/SAP/Notes/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\SAP\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F97A112-412A-43C3-9C9C-B33B4FB3CE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0406380-8756-47FF-8357-BEE8562CAD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10080" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Managerial round" sheetId="14" r:id="rId1"/>
@@ -25,13 +25,14 @@
     <sheet name="Cross-company" sheetId="8" r:id="rId10"/>
     <sheet name="STO" sheetId="9" r:id="rId11"/>
     <sheet name="OPD" sheetId="19" r:id="rId12"/>
-    <sheet name="MTS &amp; MTO" sheetId="11" r:id="rId13"/>
-    <sheet name="Others" sheetId="21" r:id="rId14"/>
-    <sheet name="Issues!." sheetId="12" r:id="rId15"/>
-    <sheet name="Custom Fiori Application" sheetId="18" r:id="rId16"/>
-    <sheet name="HANA vs ECC" sheetId="1" r:id="rId17"/>
-    <sheet name="Idoc structure" sheetId="3" r:id="rId18"/>
-    <sheet name="ALE" sheetId="10" r:id="rId19"/>
+    <sheet name="ATP" sheetId="22" r:id="rId13"/>
+    <sheet name="MTS &amp; MTO" sheetId="11" r:id="rId14"/>
+    <sheet name="Others" sheetId="21" r:id="rId15"/>
+    <sheet name="Issues!." sheetId="12" r:id="rId16"/>
+    <sheet name="Custom Fiori Application" sheetId="18" r:id="rId17"/>
+    <sheet name="HANA vs ECC" sheetId="1" r:id="rId18"/>
+    <sheet name="Idoc structure" sheetId="3" r:id="rId19"/>
+    <sheet name="ALE" sheetId="10" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="894">
   <si>
     <t>Module</t>
   </si>
@@ -5142,12 +5143,298 @@
 This account keys and accruals are assigned to respective G/L accounts. Therefore, the system posts respective values in respective G/L accounts in Fi-Co Module.
 This also one of the areas of SD - Fi Integration. SD consultants are responsible for assigning the account keys and Fi Consultants have to assign the respective G/L accounts in T.Code: VKOA.</t>
   </si>
+  <si>
+    <t>Have you worked with Workflows, Forms &amp; Outputs?</t>
+  </si>
+  <si>
+    <t>Have you worked with BPD?</t>
+  </si>
+  <si>
+    <t>BASICS</t>
+  </si>
+  <si>
+    <t>ATP= Current stock + Inward Movement(Purc. Order &amp; Plan. order)+ Outward Movement(SO+Deliveries)</t>
+  </si>
+  <si>
+    <t>ATP= Current stock + Planned Receipts + Planned Issues</t>
+  </si>
+  <si>
+    <t>On a day, where a order on Jan10 is placed for 10 Qty , Stock(100) will not go down but the ATP(will go down to 90 qty) with respect to the order on Jan10. Stock will go down to the ATP level(90 qty) only based on the PGI done for the delivery created for the order on Jan11.
+When PO is created for 10-Qty to on Jan11 which is to be received on Jan15, ATP will raise to 100 Qty for Jan15 on Jan11 itself whereas stock level will move to 100Qty only aftr the goods received on Jan15.</t>
+  </si>
+  <si>
+    <t>For Production, RLT= Current date + Prod. Time + G/R Proc. Time</t>
+  </si>
+  <si>
+    <t>For Procurement, RLT= Purc. Lead time(SPRO--&gt;MM-&gt;Purchasing-&gt;PR-&gt;Proc. time) + G/R Proc. Time(P. view of MM) + Planned Delivery time
+Purc. Lead time is the time taken by Purc. officer to convert PR to PO</t>
+  </si>
+  <si>
+    <t>Replenishment lead time(Master data for ATP) defines how long it takes to make the material available. When you can't break the RLT into different comp like Prod. Time &amp; Proc. Time, then make use of Total RLT(used if it is Internal procurement) in MRP3 view.</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Avaialabilty check Timing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> During Order creation/change; delivery; PGI</t>
+    </r>
+  </si>
+  <si>
+    <t>01- Individual requirements(requirements shared straightaway w.r.t order)- For high value products
+02- Daily requirements(requirements are collected and shared at the end of the day) - For small materials like spares etc..,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moving parts behind 
+1. AC- Checking group(Sales General/plant view)
+</t>
+  </si>
+  <si>
+    <t>2. Checking rule(defines how AC needs to be done)-</t>
+  </si>
+  <si>
+    <t>SPRO-&gt;SD-&gt;BF-&gt; AC &amp; TOR -&gt;AC-&gt; AC with ATP Logic-&gt; Define Checking Group
+* defines how the system takes into account diffe. Stock types while doing Availability check
+* can be defined at order level or delivery level</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SPRO-&gt;SD-&gt;BF-&gt; AC &amp; TOR -&gt;AC-&gt; AC with ATP Logic-&gt; Define Checking Rule
+* Specifies how stock is calculated, meaning what type of inward movement/outward movement is included
+* It is in-built and cannot be created newly
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Stocks:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. Include Safety stock--&gt; if 1000 stock is there, 500 will be added as safety stock for urgent requirements.
+2. Include Transfer--&gt; if Stock transfer needs to be included in ATP
+3. Include Qual. Ins stock--&gt; 
+4. Include blocked stock--&gt; 
+* By default, the above will not be included except for unrestricted stock
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Inward/outward movements:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>I. Include Purchase orders; Include PR; Include Sales req; Include Deliveries</t>
+    </r>
+  </si>
+  <si>
+    <t>3. SCL</t>
+  </si>
+  <si>
+    <t>5. RV03VFZZ/MV45AFZF, etc(for customization)</t>
+  </si>
+  <si>
+    <t>4. Delivery Item category</t>
+  </si>
+  <si>
+    <t>Enabling Availability check box in SCL(order level availability is controlled by SCL)</t>
+  </si>
+  <si>
+    <t>Enabling Availability check box in Delivery Item category(Delivery level availability is controlled by this)</t>
+  </si>
+  <si>
+    <t>Checking group</t>
+  </si>
+  <si>
+    <t>Also done configurations:</t>
+  </si>
+  <si>
+    <t>1. Define Maerial block for customers</t>
+  </si>
+  <si>
+    <t>2. Define check. Group default values: Mat. Type + Plant: CG</t>
+  </si>
+  <si>
+    <t>Under AC with ATP logic</t>
+  </si>
+  <si>
+    <t>3. Define procedure for each SLC: SL: AC[]+ TOR[] + ALL[]</t>
+  </si>
+  <si>
+    <t>5. Define Default values for AC for Sales Area</t>
+  </si>
+  <si>
+    <t>Indicators</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>Req. class</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>A or I</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>AC/Requirement Type Determination</t>
+  </si>
+  <si>
+    <t>Ex: If we maintain MRP type in MRP1 view as "NP-No planning", then it means it it not relevant for Procurement, then requirement type is acquired by "Item cat + MRP type=011", ie TAN + MD= 011
+If we maintain MRP type in MRP1 view as "PD-MRP", it is relevant for procurement, then RT is determined by "TAN+PD=041"</t>
+  </si>
+  <si>
+    <t>Strategy group(MRP3 view), MRP group(MRP1 view), Mat.type(FERT, HAWA), SCL, Item category(IC+MRP Type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOR </t>
+  </si>
+  <si>
+    <t>Path: SPRO--&gt; IMG--&gt; SD--&gt; BF --&gt; AC &amp; TOR--&gt; TOR</t>
+  </si>
+  <si>
+    <t>Define Requirement classes</t>
+  </si>
+  <si>
+    <t>Define Requirement types</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Delivery requirement:011--&gt; AC[y] + Req[y]</t>
+  </si>
+  <si>
+    <t>Order &amp; Delivery requirement:041--&gt; AC[y] + Req[y] + PA[y]</t>
+  </si>
+  <si>
+    <t>Will assigned to Requirement classes</t>
+  </si>
+  <si>
+    <t>Determination of Req. Types using Transaction</t>
+  </si>
+  <si>
+    <t>IC+MRP</t>
+  </si>
+  <si>
+    <t>TAN+PD=041</t>
+  </si>
+  <si>
+    <t>TAN+NP=011</t>
+  </si>
+  <si>
+    <t>Define procedure for each SLC: SL: AC[]+ TOR[] + ALL[]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. Define Procedure for Delivery Item category: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>If this is blank, it is relevant for Availability check</t>
+    </r>
+  </si>
+  <si>
+    <t>Delivery scheduling</t>
+  </si>
+  <si>
+    <t>3. TRLT--&gt; MRP3 view</t>
+  </si>
+  <si>
+    <t>2. Loading time- [A]-Route dependent --&gt; Shipping point(definition)</t>
+  </si>
+  <si>
+    <t>SPRO-&gt;IMG-&gt;SD-&gt;BF-&gt;Routes-&gt; Define Routes &amp; stages</t>
+  </si>
+  <si>
+    <t>For internal production</t>
+  </si>
+  <si>
+    <t>4.  Transit Time--&gt; count of days</t>
+  </si>
+  <si>
+    <t>5.  Transportation time--&gt; count of days</t>
+  </si>
+  <si>
+    <t>SPRO-&gt;IMG-&gt;SD-&gt;BF-&gt;Delivery scheduling--&gt; DS by Sales Document Type(OR: DS[x] &amp; Trans. Scheduling [y]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Pick/Pack time[A] Route dependent --&gt; Shipping point(definition) </t>
+  </si>
+  <si>
+    <t>SPRO-&gt;IMG-&gt;SD-&gt;BF-&gt;Delivery scheduling--&gt; DS by Shipping point(SP: Pick/pack time[A] ; Load time[A]; Rounding time[2]</t>
+  </si>
+  <si>
+    <t>Backward if MAD is same as the order date</t>
+  </si>
+  <si>
+    <t>Forward if MAD is not same as order date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5339,12 +5626,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF040C28"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF040C28"/>
       <name val="Tahoma"/>
@@ -5668,7 +5949,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -5891,11 +6172,33 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="15" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5905,21 +6208,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="15" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5966,6 +6254,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5978,22 +6272,12 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6159,6 +6443,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>90715</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6059714</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>90714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E641E12-0358-F4A4-CE92-700D37895AF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7048501"/>
+          <a:ext cx="6059714" cy="1959428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -6204,7 +6537,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -7385,134 +7718,134 @@
   <sheetFormatPr defaultRowHeight="110.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:22" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="122" t="s">
         <v>597</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="119"/>
-      <c r="P1" s="119"/>
-      <c r="Q1" s="119"/>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
-      <c r="T1" s="119"/>
-      <c r="U1" s="119"/>
-      <c r="V1" s="119"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="122"/>
+      <c r="P1" s="122"/>
+      <c r="Q1" s="122"/>
+      <c r="R1" s="122"/>
+      <c r="S1" s="122"/>
+      <c r="T1" s="122"/>
+      <c r="U1" s="122"/>
+      <c r="V1" s="122"/>
     </row>
     <row r="2" spans="1:22" ht="98" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="125" t="s">
         <v>245</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+      <c r="O2" s="125"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="125"/>
+      <c r="V2" s="125"/>
     </row>
     <row r="3" spans="1:22" ht="260" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="126" t="s">
         <v>246</v>
       </c>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="121"/>
-      <c r="O3" s="121"/>
-      <c r="P3" s="121"/>
-      <c r="Q3" s="121"/>
-      <c r="R3" s="121"/>
-      <c r="S3" s="121"/>
-      <c r="T3" s="121"/>
-      <c r="U3" s="121"/>
-      <c r="V3" s="121"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="126"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="126"/>
     </row>
     <row r="4" spans="1:22" ht="308.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="120" t="s">
+      <c r="A4" s="125" t="s">
         <v>247</v>
       </c>
-      <c r="B4" s="122"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="122"/>
-      <c r="H4" s="122"/>
-      <c r="I4" s="122"/>
-      <c r="J4" s="122"/>
-      <c r="K4" s="122"/>
-      <c r="L4" s="122"/>
-      <c r="M4" s="122"/>
-      <c r="N4" s="122"/>
-      <c r="O4" s="122"/>
-      <c r="P4" s="122"/>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="122"/>
-      <c r="S4" s="122"/>
-      <c r="T4" s="122"/>
-      <c r="U4" s="122"/>
-      <c r="V4" s="122"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="127"/>
+      <c r="N4" s="127"/>
+      <c r="O4" s="127"/>
+      <c r="P4" s="127"/>
+      <c r="Q4" s="127"/>
+      <c r="R4" s="127"/>
+      <c r="S4" s="127"/>
+      <c r="T4" s="127"/>
+      <c r="U4" s="127"/>
+      <c r="V4" s="127"/>
     </row>
     <row r="5" spans="1:22" ht="409" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="126" t="s">
         <v>248</v>
       </c>
-      <c r="B5" s="122"/>
-      <c r="C5" s="122"/>
-      <c r="D5" s="122"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="122"/>
-      <c r="G5" s="122"/>
-      <c r="H5" s="122"/>
-      <c r="I5" s="122"/>
-      <c r="J5" s="122"/>
-      <c r="K5" s="122"/>
-      <c r="L5" s="122"/>
-      <c r="M5" s="122"/>
-      <c r="N5" s="122"/>
-      <c r="O5" s="122"/>
-      <c r="P5" s="122"/>
-      <c r="Q5" s="122"/>
-      <c r="R5" s="122"/>
-      <c r="S5" s="122"/>
-      <c r="T5" s="122"/>
-      <c r="U5" s="122"/>
-      <c r="V5" s="122"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="127"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="127"/>
+      <c r="K5" s="127"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="127"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
+      <c r="Q5" s="127"/>
+      <c r="R5" s="127"/>
+      <c r="S5" s="127"/>
+      <c r="T5" s="127"/>
+      <c r="U5" s="127"/>
+      <c r="V5" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7785,6 +8118,327 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F62B76-A999-4491-9487-4664B67861D8}">
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="88.6328125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="91.36328125" style="87" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7265625" style="87" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>831</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>836</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>838</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+      <c r="A9" s="49" t="s">
+        <v>864</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="50" x14ac:dyDescent="0.25">
+      <c r="A10" s="129"/>
+      <c r="B10" s="80" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="49" t="s">
+        <v>882</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="67" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>840</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>842</v>
+      </c>
+      <c r="C14" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>856</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>857</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="137.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>841</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>843</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>859</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>860</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>844</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>847</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>862</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>860</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>846</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>848</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>860</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>845</v>
+      </c>
+      <c r="B18" s="27"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>849</v>
+      </c>
+      <c r="B22" s="130" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="130" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="27" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="27" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="74" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="27" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="27" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="95" t="s">
+        <v>867</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>868</v>
+      </c>
+      <c r="B38" s="131" t="s">
+        <v>869</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>873</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="C39" s="80" t="s">
+        <v>874</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>870</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="74" t="s">
+        <v>876</v>
+      </c>
+      <c r="C41" s="92" t="s">
+        <v>877</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>878</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="22" t="s">
+        <v>879</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="27" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>890</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>884</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
+        <v>883</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>887</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>888</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>885</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A341B7-644B-4D77-B5EC-8E37D7458E3E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -7836,7 +8490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E11BB8B-6D1A-426B-A94E-2E5CF457241F}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -7904,7 +8558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E189C3C3-EEB1-493B-8ABF-EFAFC403CD7F}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -7950,7 +8604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B651BB52-6CE9-469E-B50D-672679C49F78}">
   <dimension ref="A1:L14"/>
   <sheetViews>
@@ -8231,7 +8885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -8311,11 +8965,11 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="123" t="s">
+      <c r="A8" s="128" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="123"/>
-      <c r="C8" s="123"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
     </row>
     <row r="9" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
@@ -8371,11 +9025,11 @@
       <c r="C13" s="22"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="123" t="s">
+      <c r="A15" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="B15" s="123"/>
-      <c r="C15" s="123"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="128"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="s">
@@ -8452,7 +9106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8E8FD8-CC4D-41B5-9F85-742D913B8828}">
   <dimension ref="A1:AD120"/>
   <sheetViews>
@@ -8530,50 +9184,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8599D4-DE0E-4BD2-843B-7435980E71AE}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="114.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549ECB4F-00E1-4BF6-8909-4BA1BD6871D5}">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109:C109"/>
+    <sheetView topLeftCell="A110" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="255.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8618,13 +9234,13 @@
       <c r="C2" s="27" t="s">
         <v>456</v>
       </c>
-      <c r="D2" s="96" t="s">
+      <c r="D2" s="99" t="s">
         <v>457</v>
       </c>
-      <c r="E2" s="104">
+      <c r="E2" s="101">
         <v>44436</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="104" t="s">
         <v>458</v>
       </c>
     </row>
@@ -8638,9 +9254,9 @@
       <c r="C3" s="83" t="s">
         <v>775</v>
       </c>
-      <c r="D3" s="95"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="84" t="s">
@@ -8652,9 +9268,9 @@
       <c r="C4" s="86" t="s">
         <v>461</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
@@ -8666,9 +9282,9 @@
       <c r="C5" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="D5" s="95"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
@@ -8680,9 +9296,9 @@
       <c r="C6" s="27" t="s">
         <v>466</v>
       </c>
-      <c r="D6" s="95"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
@@ -8694,9 +9310,9 @@
       <c r="C7" s="27" t="s">
         <v>468</v>
       </c>
-      <c r="D7" s="95"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="101"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -8708,9 +9324,9 @@
       <c r="C8" s="85" t="s">
         <v>470</v>
       </c>
-      <c r="D8" s="95"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
@@ -8722,9 +9338,9 @@
       <c r="C9" s="22" t="s">
         <v>472</v>
       </c>
-      <c r="D9" s="95"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
     </row>
     <row r="10" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
@@ -8734,9 +9350,9 @@
       <c r="C10" s="27" t="s">
         <v>474</v>
       </c>
-      <c r="D10" s="95"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="84" t="s">
@@ -8748,9 +9364,9 @@
       <c r="C11" s="27" t="s">
         <v>594</v>
       </c>
-      <c r="D11" s="95"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
     </row>
     <row r="12" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="84" t="s">
@@ -8762,9 +9378,9 @@
       <c r="C12" s="27" t="s">
         <v>776</v>
       </c>
-      <c r="D12" s="95"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
@@ -8774,9 +9390,9 @@
         <v>463</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="84" t="s">
@@ -8788,9 +9404,9 @@
       <c r="C14" s="22" t="s">
         <v>479</v>
       </c>
-      <c r="D14" s="95"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
@@ -8802,9 +9418,9 @@
       <c r="C15" s="22" t="s">
         <v>481</v>
       </c>
-      <c r="D15" s="95"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="102"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
@@ -8816,9 +9432,9 @@
       <c r="C16" s="22" t="s">
         <v>483</v>
       </c>
-      <c r="D16" s="95"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
@@ -8830,9 +9446,9 @@
       <c r="C17" s="22" t="s">
         <v>485</v>
       </c>
-      <c r="D17" s="95"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
     </row>
     <row r="18" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A18" s="84" t="s">
@@ -8844,9 +9460,9 @@
       <c r="C18" s="87" t="s">
         <v>777</v>
       </c>
-      <c r="D18" s="95"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="84" t="s">
@@ -8858,9 +9474,9 @@
       <c r="C19" s="22" t="s">
         <v>488</v>
       </c>
-      <c r="D19" s="95"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="101"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="102"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
@@ -8872,9 +9488,9 @@
       <c r="C20" s="22" t="s">
         <v>490</v>
       </c>
-      <c r="D20" s="95"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
     </row>
     <row r="21" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A21" s="84" t="s">
@@ -8886,9 +9502,9 @@
       <c r="C21" s="27" t="s">
         <v>492</v>
       </c>
-      <c r="D21" s="95"/>
-      <c r="E21" s="101"/>
-      <c r="F21" s="101"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
     </row>
     <row r="22" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A22" s="84" t="s">
@@ -8900,9 +9516,9 @@
       <c r="C22" s="27" t="s">
         <v>494</v>
       </c>
-      <c r="D22" s="95"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="103"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23" s="81"/>
@@ -8928,13 +9544,13 @@
       <c r="C25" s="88" t="s">
         <v>497</v>
       </c>
-      <c r="D25" s="95" t="s">
+      <c r="D25" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="E25" s="96" t="s">
+      <c r="E25" s="99" t="s">
         <v>499</v>
       </c>
-      <c r="F25" s="96" t="s">
+      <c r="F25" s="99" t="s">
         <v>500</v>
       </c>
     </row>
@@ -8948,9 +9564,9 @@
       <c r="C26" s="88" t="s">
         <v>502</v>
       </c>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="96"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="99"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="89" t="s">
@@ -8962,9 +9578,9 @@
       <c r="C27" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="96"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="100"/>
+      <c r="F27" s="99"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -8976,9 +9592,9 @@
       <c r="C28" s="90" t="s">
         <v>505</v>
       </c>
-      <c r="D28" s="95"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="96"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="99"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="89" t="s">
@@ -8990,9 +9606,9 @@
       <c r="C29" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="96"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="99"/>
     </row>
     <row r="30" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A30" s="89" t="s">
@@ -9004,9 +9620,9 @@
       <c r="C30" s="72" t="s">
         <v>507</v>
       </c>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="96"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="100"/>
+      <c r="F30" s="99"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="89" t="s">
@@ -9018,9 +9634,9 @@
       <c r="C31" s="22" t="s">
         <v>509</v>
       </c>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="96"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="99"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -9032,9 +9648,9 @@
       <c r="C32" s="88" t="s">
         <v>511</v>
       </c>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="96"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="100"/>
+      <c r="F32" s="99"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
@@ -9046,9 +9662,9 @@
       <c r="C33" s="88" t="s">
         <v>513</v>
       </c>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="96"/>
+      <c r="D33" s="100"/>
+      <c r="E33" s="100"/>
+      <c r="F33" s="99"/>
     </row>
     <row r="34" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
@@ -9060,9 +9676,9 @@
       <c r="C34" s="72" t="s">
         <v>515</v>
       </c>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="96"/>
+      <c r="D34" s="100"/>
+      <c r="E34" s="100"/>
+      <c r="F34" s="99"/>
     </row>
     <row r="35" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A35" s="84" t="s">
@@ -9074,9 +9690,9 @@
       <c r="C35" s="72" t="s">
         <v>518</v>
       </c>
-      <c r="D35" s="95"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="96"/>
+      <c r="D35" s="100"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="99"/>
       <c r="G35" s="91" t="s">
         <v>595</v>
       </c>
@@ -9091,9 +9707,9 @@
       <c r="C36" s="88" t="s">
         <v>520</v>
       </c>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="96"/>
+      <c r="D36" s="100"/>
+      <c r="E36" s="100"/>
+      <c r="F36" s="99"/>
       <c r="G36" s="20" t="s">
         <v>596</v>
       </c>
@@ -9108,9 +9724,9 @@
       <c r="C37" s="88" t="s">
         <v>523</v>
       </c>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="96"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="99"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="84" t="s">
@@ -9122,9 +9738,9 @@
       <c r="C38" s="88" t="s">
         <v>525</v>
       </c>
-      <c r="D38" s="95"/>
-      <c r="E38" s="95"/>
-      <c r="F38" s="96"/>
+      <c r="D38" s="100"/>
+      <c r="E38" s="100"/>
+      <c r="F38" s="99"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
@@ -9134,9 +9750,9 @@
         <v>463</v>
       </c>
       <c r="C39" s="88"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="96"/>
+      <c r="D39" s="100"/>
+      <c r="E39" s="100"/>
+      <c r="F39" s="99"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
@@ -9148,9 +9764,9 @@
       <c r="C40" s="88" t="s">
         <v>528</v>
       </c>
-      <c r="D40" s="95"/>
-      <c r="E40" s="95"/>
-      <c r="F40" s="96"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="100"/>
+      <c r="F40" s="99"/>
     </row>
     <row r="41" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
@@ -9162,9 +9778,9 @@
       <c r="C41" s="72" t="s">
         <v>530</v>
       </c>
-      <c r="D41" s="95"/>
-      <c r="E41" s="95"/>
-      <c r="F41" s="96"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="99"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
@@ -9176,9 +9792,9 @@
       <c r="C42" s="88" t="s">
         <v>533</v>
       </c>
-      <c r="D42" s="95"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="96"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="99"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
@@ -9200,13 +9816,13 @@
       <c r="C45" s="92" t="s">
         <v>536</v>
       </c>
-      <c r="D45" s="100" t="s">
+      <c r="D45" s="104" t="s">
         <v>537</v>
       </c>
-      <c r="E45" s="97" t="s">
+      <c r="E45" s="105" t="s">
         <v>538</v>
       </c>
-      <c r="F45" s="100" t="s">
+      <c r="F45" s="104" t="s">
         <v>458</v>
       </c>
     </row>
@@ -9220,9 +9836,9 @@
       <c r="C46" s="78" t="s">
         <v>540</v>
       </c>
-      <c r="D46" s="101"/>
-      <c r="E46" s="98"/>
-      <c r="F46" s="101"/>
+      <c r="D46" s="102"/>
+      <c r="E46" s="106"/>
+      <c r="F46" s="102"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
@@ -9234,9 +9850,9 @@
       <c r="C47" s="78" t="s">
         <v>542</v>
       </c>
-      <c r="D47" s="101"/>
-      <c r="E47" s="98"/>
-      <c r="F47" s="101"/>
+      <c r="D47" s="102"/>
+      <c r="E47" s="106"/>
+      <c r="F47" s="102"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -9246,9 +9862,9 @@
         <v>532</v>
       </c>
       <c r="C48" s="78"/>
-      <c r="D48" s="101"/>
-      <c r="E48" s="98"/>
-      <c r="F48" s="101"/>
+      <c r="D48" s="102"/>
+      <c r="E48" s="106"/>
+      <c r="F48" s="102"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
@@ -9260,9 +9876,9 @@
       <c r="C49" s="78" t="s">
         <v>545</v>
       </c>
-      <c r="D49" s="101"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="101"/>
+      <c r="D49" s="102"/>
+      <c r="E49" s="106"/>
+      <c r="F49" s="102"/>
     </row>
     <row r="50" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
@@ -9274,9 +9890,9 @@
       <c r="C50" s="92" t="s">
         <v>547</v>
       </c>
-      <c r="D50" s="101"/>
-      <c r="E50" s="98"/>
-      <c r="F50" s="101"/>
+      <c r="D50" s="102"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="102"/>
     </row>
     <row r="51" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
@@ -9288,9 +9904,9 @@
       <c r="C51" s="92" t="s">
         <v>549</v>
       </c>
-      <c r="D51" s="101"/>
-      <c r="E51" s="98"/>
-      <c r="F51" s="101"/>
+      <c r="D51" s="102"/>
+      <c r="E51" s="106"/>
+      <c r="F51" s="102"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
@@ -9300,9 +9916,9 @@
         <v>455</v>
       </c>
       <c r="C52" s="78"/>
-      <c r="D52" s="101"/>
-      <c r="E52" s="98"/>
-      <c r="F52" s="101"/>
+      <c r="D52" s="102"/>
+      <c r="E52" s="106"/>
+      <c r="F52" s="102"/>
     </row>
     <row r="53" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
@@ -9314,9 +9930,9 @@
       <c r="C53" s="92" t="s">
         <v>552</v>
       </c>
-      <c r="D53" s="101"/>
-      <c r="E53" s="98"/>
-      <c r="F53" s="101"/>
+      <c r="D53" s="102"/>
+      <c r="E53" s="106"/>
+      <c r="F53" s="102"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
@@ -9326,9 +9942,9 @@
         <v>455</v>
       </c>
       <c r="C54" s="78"/>
-      <c r="D54" s="101"/>
-      <c r="E54" s="98"/>
-      <c r="F54" s="101"/>
+      <c r="D54" s="102"/>
+      <c r="E54" s="106"/>
+      <c r="F54" s="102"/>
     </row>
     <row r="55" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
@@ -9340,9 +9956,9 @@
       <c r="C55" s="93" t="s">
         <v>778</v>
       </c>
-      <c r="D55" s="102"/>
-      <c r="E55" s="99"/>
-      <c r="F55" s="102"/>
+      <c r="D55" s="103"/>
+      <c r="E55" s="107"/>
+      <c r="F55" s="103"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="25"/>
@@ -9362,11 +9978,11 @@
       <c r="C57" s="72" t="s">
         <v>556</v>
       </c>
-      <c r="D57" s="95" t="s">
+      <c r="D57" s="100" t="s">
         <v>557</v>
       </c>
-      <c r="E57" s="105"/>
-      <c r="F57" s="100" t="s">
+      <c r="E57" s="108"/>
+      <c r="F57" s="104" t="s">
         <v>558</v>
       </c>
     </row>
@@ -9380,9 +9996,9 @@
       <c r="C58" s="27" t="s">
         <v>560</v>
       </c>
-      <c r="D58" s="95"/>
-      <c r="E58" s="105"/>
-      <c r="F58" s="101"/>
+      <c r="D58" s="100"/>
+      <c r="E58" s="108"/>
+      <c r="F58" s="102"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
@@ -9394,9 +10010,9 @@
       <c r="C59" s="22" t="s">
         <v>562</v>
       </c>
-      <c r="D59" s="95"/>
-      <c r="E59" s="105"/>
-      <c r="F59" s="101"/>
+      <c r="D59" s="100"/>
+      <c r="E59" s="108"/>
+      <c r="F59" s="102"/>
     </row>
     <row r="60" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A60" s="89" t="s">
@@ -9408,9 +10024,9 @@
       <c r="C60" s="94" t="s">
         <v>547</v>
       </c>
-      <c r="D60" s="95"/>
-      <c r="E60" s="105"/>
-      <c r="F60" s="101"/>
+      <c r="D60" s="100"/>
+      <c r="E60" s="108"/>
+      <c r="F60" s="102"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
@@ -9422,9 +10038,9 @@
       <c r="C61" s="22" t="s">
         <v>565</v>
       </c>
-      <c r="D61" s="95"/>
-      <c r="E61" s="105"/>
-      <c r="F61" s="101"/>
+      <c r="D61" s="100"/>
+      <c r="E61" s="108"/>
+      <c r="F61" s="102"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
@@ -9436,9 +10052,9 @@
       <c r="C62" s="22" t="s">
         <v>565</v>
       </c>
-      <c r="D62" s="95"/>
-      <c r="E62" s="105"/>
-      <c r="F62" s="102"/>
+      <c r="D62" s="100"/>
+      <c r="E62" s="108"/>
+      <c r="F62" s="103"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="25"/>
@@ -9458,13 +10074,13 @@
       <c r="C64" s="22" t="s">
         <v>568</v>
       </c>
-      <c r="D64" s="95" t="s">
+      <c r="D64" s="100" t="s">
         <v>569</v>
       </c>
-      <c r="E64" s="96" t="s">
+      <c r="E64" s="99" t="s">
         <v>570</v>
       </c>
-      <c r="F64" s="96" t="s">
+      <c r="F64" s="99" t="s">
         <v>571</v>
       </c>
     </row>
@@ -9478,9 +10094,9 @@
       <c r="C65" s="94" t="s">
         <v>547</v>
       </c>
-      <c r="D65" s="95"/>
-      <c r="E65" s="95"/>
-      <c r="F65" s="95"/>
+      <c r="D65" s="100"/>
+      <c r="E65" s="100"/>
+      <c r="F65" s="100"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
@@ -9492,9 +10108,9 @@
       <c r="C66" s="22" t="s">
         <v>523</v>
       </c>
-      <c r="D66" s="95"/>
-      <c r="E66" s="95"/>
-      <c r="F66" s="95"/>
+      <c r="D66" s="100"/>
+      <c r="E66" s="100"/>
+      <c r="F66" s="100"/>
     </row>
     <row r="67" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A67" s="22" t="s">
@@ -9506,9 +10122,9 @@
       <c r="C67" s="27" t="s">
         <v>779</v>
       </c>
-      <c r="D67" s="95"/>
-      <c r="E67" s="95"/>
-      <c r="F67" s="95"/>
+      <c r="D67" s="100"/>
+      <c r="E67" s="100"/>
+      <c r="F67" s="100"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="s">
@@ -9520,9 +10136,9 @@
       <c r="C68" s="22" t="s">
         <v>523</v>
       </c>
-      <c r="D68" s="95"/>
-      <c r="E68" s="95"/>
-      <c r="F68" s="95"/>
+      <c r="D68" s="100"/>
+      <c r="E68" s="100"/>
+      <c r="F68" s="100"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="25"/>
@@ -9538,13 +10154,13 @@
       </c>
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
-      <c r="D70" s="97" t="s">
+      <c r="D70" s="105" t="s">
         <v>576</v>
       </c>
-      <c r="E70" s="97" t="s">
+      <c r="E70" s="105" t="s">
         <v>577</v>
       </c>
-      <c r="F70" s="100" t="s">
+      <c r="F70" s="104" t="s">
         <v>578</v>
       </c>
     </row>
@@ -9554,9 +10170,9 @@
       </c>
       <c r="B71" s="22"/>
       <c r="C71" s="22"/>
-      <c r="D71" s="98"/>
-      <c r="E71" s="98"/>
-      <c r="F71" s="101"/>
+      <c r="D71" s="106"/>
+      <c r="E71" s="106"/>
+      <c r="F71" s="102"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="22" t="s">
@@ -9564,9 +10180,9 @@
       </c>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
-      <c r="D72" s="98"/>
-      <c r="E72" s="98"/>
-      <c r="F72" s="101"/>
+      <c r="D72" s="106"/>
+      <c r="E72" s="106"/>
+      <c r="F72" s="102"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
@@ -9574,17 +10190,17 @@
       </c>
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
-      <c r="D73" s="99"/>
-      <c r="E73" s="99"/>
-      <c r="F73" s="102"/>
+      <c r="D73" s="107"/>
+      <c r="E73" s="107"/>
+      <c r="F73" s="103"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="106"/>
-      <c r="B74" s="107"/>
-      <c r="C74" s="107"/>
-      <c r="D74" s="107"/>
-      <c r="E74" s="107"/>
-      <c r="F74" s="108"/>
+      <c r="A74" s="109"/>
+      <c r="B74" s="110"/>
+      <c r="C74" s="110"/>
+      <c r="D74" s="110"/>
+      <c r="E74" s="110"/>
+      <c r="F74" s="111"/>
     </row>
     <row r="75" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A75" s="89" t="s">
@@ -9596,11 +10212,11 @@
       <c r="C75" s="94" t="s">
         <v>547</v>
       </c>
-      <c r="D75" s="95"/>
-      <c r="E75" s="96" t="s">
+      <c r="D75" s="100"/>
+      <c r="E75" s="99" t="s">
         <v>583</v>
       </c>
-      <c r="F75" s="95" t="s">
+      <c r="F75" s="100" t="s">
         <v>584</v>
       </c>
     </row>
@@ -9614,9 +10230,9 @@
       <c r="C76" s="22" t="s">
         <v>586</v>
       </c>
-      <c r="D76" s="95"/>
-      <c r="E76" s="95"/>
-      <c r="F76" s="95"/>
+      <c r="D76" s="100"/>
+      <c r="E76" s="100"/>
+      <c r="F76" s="100"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="22" t="s">
@@ -9628,9 +10244,9 @@
       <c r="C77" s="22" t="s">
         <v>588</v>
       </c>
-      <c r="D77" s="95"/>
-      <c r="E77" s="95"/>
-      <c r="F77" s="95"/>
+      <c r="D77" s="100"/>
+      <c r="E77" s="100"/>
+      <c r="F77" s="100"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="22" t="s">
@@ -9642,9 +10258,9 @@
       <c r="C78" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="D78" s="95"/>
-      <c r="E78" s="95"/>
-      <c r="F78" s="95"/>
+      <c r="D78" s="100"/>
+      <c r="E78" s="100"/>
+      <c r="F78" s="100"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="89" t="s">
@@ -9656,9 +10272,9 @@
       <c r="C79" s="94" t="s">
         <v>592</v>
       </c>
-      <c r="D79" s="95"/>
-      <c r="E79" s="95"/>
-      <c r="F79" s="95"/>
+      <c r="D79" s="100"/>
+      <c r="E79" s="100"/>
+      <c r="F79" s="100"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="22" t="s">
@@ -9688,7 +10304,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="124" t="s">
+      <c r="A85" s="95" t="s">
         <v>794</v>
       </c>
     </row>
@@ -9702,13 +10318,13 @@
       <c r="C86" s="22" t="s">
         <v>643</v>
       </c>
-      <c r="D86" s="103" t="s">
+      <c r="D86" s="98" t="s">
         <v>569</v>
       </c>
-      <c r="E86" s="96" t="s">
+      <c r="E86" s="99" t="s">
         <v>652</v>
       </c>
-      <c r="F86" s="103" t="s">
+      <c r="F86" s="98" t="s">
         <v>458</v>
       </c>
     </row>
@@ -9722,9 +10338,9 @@
       <c r="C87" s="22" t="s">
         <v>645</v>
       </c>
-      <c r="D87" s="103"/>
-      <c r="E87" s="96"/>
-      <c r="F87" s="103"/>
+      <c r="D87" s="98"/>
+      <c r="E87" s="99"/>
+      <c r="F87" s="98"/>
     </row>
     <row r="88" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A88" s="22" t="s">
@@ -9736,9 +10352,9 @@
       <c r="C88" s="27" t="s">
         <v>657</v>
       </c>
-      <c r="D88" s="103"/>
-      <c r="E88" s="96"/>
-      <c r="F88" s="103"/>
+      <c r="D88" s="98"/>
+      <c r="E88" s="99"/>
+      <c r="F88" s="98"/>
     </row>
     <row r="89" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A89" s="22" t="s">
@@ -9750,9 +10366,9 @@
       <c r="C89" s="27" t="s">
         <v>659</v>
       </c>
-      <c r="D89" s="103"/>
-      <c r="E89" s="96"/>
-      <c r="F89" s="103"/>
+      <c r="D89" s="98"/>
+      <c r="E89" s="99"/>
+      <c r="F89" s="98"/>
     </row>
     <row r="90" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A90" s="22" t="s">
@@ -9764,9 +10380,9 @@
       <c r="C90" s="27" t="s">
         <v>660</v>
       </c>
-      <c r="D90" s="103"/>
-      <c r="E90" s="96"/>
-      <c r="F90" s="103"/>
+      <c r="D90" s="98"/>
+      <c r="E90" s="99"/>
+      <c r="F90" s="98"/>
     </row>
     <row r="91" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A91" s="22" t="s">
@@ -9778,9 +10394,9 @@
       <c r="C91" s="27" t="s">
         <v>656</v>
       </c>
-      <c r="D91" s="103"/>
-      <c r="E91" s="96"/>
-      <c r="F91" s="103"/>
+      <c r="D91" s="98"/>
+      <c r="E91" s="99"/>
+      <c r="F91" s="98"/>
     </row>
     <row r="92" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A92" s="22" t="s">
@@ -9792,9 +10408,9 @@
       <c r="C92" s="27" t="s">
         <v>661</v>
       </c>
-      <c r="D92" s="103"/>
-      <c r="E92" s="96"/>
-      <c r="F92" s="103"/>
+      <c r="D92" s="98"/>
+      <c r="E92" s="99"/>
+      <c r="F92" s="98"/>
     </row>
     <row r="93" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A93" s="22" t="s">
@@ -9806,12 +10422,12 @@
       <c r="C93" s="27" t="s">
         <v>658</v>
       </c>
-      <c r="D93" s="103"/>
-      <c r="E93" s="96"/>
-      <c r="F93" s="103"/>
+      <c r="D93" s="98"/>
+      <c r="E93" s="99"/>
+      <c r="F93" s="98"/>
     </row>
     <row r="95" spans="1:6" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A95" s="124" t="s">
+      <c r="A95" s="95" t="s">
         <v>793</v>
       </c>
     </row>
@@ -9823,13 +10439,13 @@
         <v>463</v>
       </c>
       <c r="C96" s="22"/>
-      <c r="D96" s="103" t="s">
+      <c r="D96" s="98" t="s">
         <v>808</v>
       </c>
-      <c r="E96" s="103" t="s">
+      <c r="E96" s="98" t="s">
         <v>809</v>
       </c>
-      <c r="F96" s="103" t="s">
+      <c r="F96" s="98" t="s">
         <v>812</v>
       </c>
     </row>
@@ -9843,9 +10459,9 @@
       <c r="C97" s="22" t="s">
         <v>813</v>
       </c>
-      <c r="D97" s="103"/>
-      <c r="E97" s="103"/>
-      <c r="F97" s="103"/>
+      <c r="D97" s="98"/>
+      <c r="E97" s="98"/>
+      <c r="F97" s="98"/>
     </row>
     <row r="98" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A98" s="22" t="s">
@@ -9857,9 +10473,9 @@
       <c r="C98" s="27" t="s">
         <v>706</v>
       </c>
-      <c r="D98" s="103"/>
-      <c r="E98" s="103"/>
-      <c r="F98" s="103"/>
+      <c r="D98" s="98"/>
+      <c r="E98" s="98"/>
+      <c r="F98" s="98"/>
     </row>
     <row r="99" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A99" s="22" t="s">
@@ -9871,9 +10487,9 @@
       <c r="C99" s="27" t="s">
         <v>815</v>
       </c>
-      <c r="D99" s="103"/>
-      <c r="E99" s="103"/>
-      <c r="F99" s="103"/>
+      <c r="D99" s="98"/>
+      <c r="E99" s="98"/>
+      <c r="F99" s="98"/>
     </row>
     <row r="100" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="22" t="s">
@@ -9885,9 +10501,9 @@
       <c r="C100" s="22" t="s">
         <v>816</v>
       </c>
-      <c r="D100" s="103"/>
-      <c r="E100" s="103"/>
-      <c r="F100" s="103"/>
+      <c r="D100" s="98"/>
+      <c r="E100" s="98"/>
+      <c r="F100" s="98"/>
     </row>
     <row r="101" spans="1:6" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="22" t="s">
@@ -9899,9 +10515,9 @@
       <c r="C101" s="22" t="s">
         <v>817</v>
       </c>
-      <c r="D101" s="103"/>
-      <c r="E101" s="103"/>
-      <c r="F101" s="103"/>
+      <c r="D101" s="98"/>
+      <c r="E101" s="98"/>
+      <c r="F101" s="98"/>
     </row>
     <row r="102" spans="1:6" ht="50" x14ac:dyDescent="0.25">
       <c r="A102" s="22" t="s">
@@ -9913,9 +10529,9 @@
       <c r="C102" s="87" t="s">
         <v>818</v>
       </c>
-      <c r="D102" s="103"/>
-      <c r="E102" s="103"/>
-      <c r="F102" s="103"/>
+      <c r="D102" s="98"/>
+      <c r="E102" s="98"/>
+      <c r="F102" s="98"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="22" t="s">
@@ -9925,9 +10541,9 @@
         <v>463</v>
       </c>
       <c r="C103" s="22"/>
-      <c r="D103" s="103"/>
-      <c r="E103" s="103"/>
-      <c r="F103" s="103"/>
+      <c r="D103" s="98"/>
+      <c r="E103" s="98"/>
+      <c r="F103" s="98"/>
     </row>
     <row r="104" spans="1:6" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A104" s="22" t="s">
@@ -9939,9 +10555,9 @@
       <c r="C104" s="27" t="s">
         <v>819</v>
       </c>
-      <c r="D104" s="103"/>
-      <c r="E104" s="103"/>
-      <c r="F104" s="103"/>
+      <c r="D104" s="98"/>
+      <c r="E104" s="98"/>
+      <c r="F104" s="98"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="22" t="s">
@@ -9953,9 +10569,9 @@
       <c r="C105" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="D105" s="103"/>
-      <c r="E105" s="103"/>
-      <c r="F105" s="103"/>
+      <c r="D105" s="98"/>
+      <c r="E105" s="98"/>
+      <c r="F105" s="98"/>
     </row>
     <row r="106" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A106" s="22" t="s">
@@ -9967,9 +10583,9 @@
       <c r="C106" s="27" t="s">
         <v>822</v>
       </c>
-      <c r="D106" s="103"/>
-      <c r="E106" s="103"/>
-      <c r="F106" s="103"/>
+      <c r="D106" s="98"/>
+      <c r="E106" s="98"/>
+      <c r="F106" s="98"/>
     </row>
     <row r="107" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A107" s="22" t="s">
@@ -9978,14 +10594,14 @@
       <c r="B107" s="22" t="s">
         <v>517</v>
       </c>
-      <c r="C107" s="129" t="s">
+      <c r="C107" s="96" t="s">
         <v>823</v>
       </c>
-      <c r="D107" s="103"/>
-      <c r="E107" s="103"/>
-      <c r="F107" s="103"/>
-    </row>
-    <row r="108" spans="1:6" ht="125" x14ac:dyDescent="0.25">
+      <c r="D107" s="98"/>
+      <c r="E107" s="98"/>
+      <c r="F107" s="98"/>
+    </row>
+    <row r="108" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A108" s="22" t="s">
         <v>802</v>
       </c>
@@ -9995,9 +10611,9 @@
       <c r="C108" s="27" t="s">
         <v>824</v>
       </c>
-      <c r="D108" s="103"/>
-      <c r="E108" s="103"/>
-      <c r="F108" s="103"/>
+      <c r="D108" s="98"/>
+      <c r="E108" s="98"/>
+      <c r="F108" s="98"/>
     </row>
     <row r="109" spans="1:6" ht="249.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="22" t="s">
@@ -10009,9 +10625,9 @@
       <c r="C109" s="27" t="s">
         <v>825</v>
       </c>
-      <c r="D109" s="103"/>
-      <c r="E109" s="103"/>
-      <c r="F109" s="103"/>
+      <c r="D109" s="98"/>
+      <c r="E109" s="98"/>
+      <c r="F109" s="98"/>
     </row>
     <row r="110" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A110" s="22" t="s">
@@ -10020,12 +10636,12 @@
       <c r="B110" s="22" t="s">
         <v>517</v>
       </c>
-      <c r="C110" s="130" t="s">
+      <c r="C110" s="97" t="s">
         <v>826</v>
       </c>
-      <c r="D110" s="103"/>
-      <c r="E110" s="103"/>
-      <c r="F110" s="103"/>
+      <c r="D110" s="98"/>
+      <c r="E110" s="98"/>
+      <c r="F110" s="98"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="22" t="s">
@@ -10035,44 +10651,50 @@
         <v>455</v>
       </c>
       <c r="C111" s="22"/>
-      <c r="D111" s="103"/>
-      <c r="E111" s="103"/>
-      <c r="F111" s="103"/>
-    </row>
-    <row r="112" spans="1:6" ht="128.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D111" s="98"/>
+      <c r="E111" s="98"/>
+      <c r="F111" s="98"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="22" t="s">
+        <v>828</v>
+      </c>
+      <c r="B112" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="C112" s="22"/>
+      <c r="D112" s="98"/>
+      <c r="E112" s="98"/>
+      <c r="F112" s="98"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="22" t="s">
+        <v>829</v>
+      </c>
+      <c r="B113" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="C113" s="22"/>
+      <c r="D113" s="98"/>
+      <c r="E113" s="98"/>
+      <c r="F113" s="98"/>
+    </row>
+    <row r="114" spans="1:6" ht="128.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="22" t="s">
         <v>811</v>
       </c>
-      <c r="B112" s="22" t="s">
+      <c r="B114" s="22" t="s">
         <v>463</v>
       </c>
-      <c r="C112" s="130" t="s">
+      <c r="C114" s="97" t="s">
         <v>827</v>
       </c>
-      <c r="D112" s="103"/>
-      <c r="E112" s="103"/>
-      <c r="F112" s="103"/>
+      <c r="D114" s="98"/>
+      <c r="E114" s="98"/>
+      <c r="F114" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D96:D112"/>
-    <mergeCell ref="E96:E112"/>
-    <mergeCell ref="F96:F112"/>
-    <mergeCell ref="D86:D93"/>
-    <mergeCell ref="E86:E93"/>
-    <mergeCell ref="F86:F93"/>
-    <mergeCell ref="D2:D22"/>
-    <mergeCell ref="E2:E22"/>
-    <mergeCell ref="F2:F22"/>
-    <mergeCell ref="D25:D42"/>
-    <mergeCell ref="E25:E42"/>
-    <mergeCell ref="F25:F42"/>
-    <mergeCell ref="D45:D55"/>
-    <mergeCell ref="E45:E55"/>
-    <mergeCell ref="F45:F55"/>
-    <mergeCell ref="D57:D62"/>
-    <mergeCell ref="E57:E62"/>
-    <mergeCell ref="F57:F62"/>
     <mergeCell ref="A74:F74"/>
     <mergeCell ref="D75:D79"/>
     <mergeCell ref="E75:E79"/>
@@ -10083,12 +10705,68 @@
     <mergeCell ref="D70:D73"/>
     <mergeCell ref="E70:E73"/>
     <mergeCell ref="F70:F73"/>
+    <mergeCell ref="D45:D55"/>
+    <mergeCell ref="E45:E55"/>
+    <mergeCell ref="F45:F55"/>
+    <mergeCell ref="D57:D62"/>
+    <mergeCell ref="E57:E62"/>
+    <mergeCell ref="F57:F62"/>
+    <mergeCell ref="D2:D22"/>
+    <mergeCell ref="E2:E22"/>
+    <mergeCell ref="F2:F22"/>
+    <mergeCell ref="D25:D42"/>
+    <mergeCell ref="E25:E42"/>
+    <mergeCell ref="F25:F42"/>
+    <mergeCell ref="D96:D114"/>
+    <mergeCell ref="E96:E114"/>
+    <mergeCell ref="F96:F114"/>
+    <mergeCell ref="D86:D93"/>
+    <mergeCell ref="E86:E93"/>
+    <mergeCell ref="F86:F93"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G35" r:id="rId1" display="https://www.stechies.com/pricing-procedure/" xr:uid="{9765D288-3CB9-4F22-BCBB-5452B93F42FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8599D4-DE0E-4BD2-843B-7435980E71AE}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="114.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12687,10 +13365,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="30"/>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="115" t="s">
         <v>353</v>
       </c>
-      <c r="C1" s="113"/>
+      <c r="C1" s="116"/>
     </row>
     <row r="2" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
@@ -12778,7 +13456,7 @@
       <c r="B11" s="39"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="117" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="40" t="s">
@@ -12789,7 +13467,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="115"/>
+      <c r="A13" s="118"/>
       <c r="B13" s="42" t="s">
         <v>371</v>
       </c>
@@ -12798,7 +13476,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="115"/>
+      <c r="A14" s="118"/>
       <c r="B14" s="44" t="s">
         <v>372</v>
       </c>
@@ -12807,7 +13485,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="115"/>
+      <c r="A15" s="118"/>
       <c r="B15" s="44" t="s">
         <v>373</v>
       </c>
@@ -12816,7 +13494,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="116"/>
+      <c r="A16" s="119"/>
       <c r="B16" s="45" t="s">
         <v>356</v>
       </c>
@@ -12833,7 +13511,7 @@
       <c r="B18" s="39"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="109" t="s">
+      <c r="A19" s="112" t="s">
         <v>375</v>
       </c>
       <c r="B19" s="47" t="s">
@@ -12844,7 +13522,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="110"/>
+      <c r="A20" s="113"/>
       <c r="B20" s="48" t="s">
         <v>377</v>
       </c>
@@ -12853,7 +13531,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="110"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="48" t="s">
         <v>378</v>
       </c>
@@ -12862,7 +13540,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="117"/>
+      <c r="A22" s="120"/>
       <c r="B22" s="48" t="s">
         <v>380</v>
       </c>
@@ -12871,7 +13549,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="117"/>
+      <c r="A23" s="120"/>
       <c r="B23" s="48" t="s">
         <v>381</v>
       </c>
@@ -12880,7 +13558,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="110"/>
+      <c r="A24" s="113"/>
       <c r="B24" s="48" t="s">
         <v>382</v>
       </c>
@@ -12889,7 +13567,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="110"/>
+      <c r="A25" s="113"/>
       <c r="B25" s="48" t="s">
         <v>384</v>
       </c>
@@ -12898,7 +13576,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="110"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="48" t="s">
         <v>385</v>
       </c>
@@ -12907,7 +13585,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="117"/>
+      <c r="A27" s="120"/>
       <c r="B27" s="48" t="s">
         <v>387</v>
       </c>
@@ -12916,7 +13594,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="118"/>
+      <c r="A28" s="121"/>
       <c r="B28" s="50" t="s">
         <v>388</v>
       </c>
@@ -12933,7 +13611,7 @@
       <c r="B30" s="39"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="109" t="s">
+      <c r="A31" s="112" t="s">
         <v>390</v>
       </c>
       <c r="B31" s="48" t="s">
@@ -12944,7 +13622,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="117"/>
+      <c r="A32" s="120"/>
       <c r="B32" s="48" t="s">
         <v>370</v>
       </c>
@@ -12953,7 +13631,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="117"/>
+      <c r="A33" s="120"/>
       <c r="B33" s="48" t="s">
         <v>394</v>
       </c>
@@ -12962,7 +13640,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="110"/>
+      <c r="A34" s="113"/>
       <c r="B34" s="48" t="s">
         <v>372</v>
       </c>
@@ -12971,7 +13649,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="111"/>
+      <c r="A35" s="114"/>
       <c r="B35" s="48" t="s">
         <v>373</v>
       </c>
@@ -13018,7 +13696,7 @@
       <c r="B41" s="39"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="109" t="s">
+      <c r="A42" s="112" t="s">
         <v>401</v>
       </c>
       <c r="B42" s="32" t="s">
@@ -13029,7 +13707,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="111"/>
+      <c r="A43" s="114"/>
       <c r="B43" s="32" t="s">
         <v>402</v>
       </c>
@@ -13046,7 +13724,7 @@
       <c r="B45" s="39"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="109" t="s">
+      <c r="A46" s="112" t="s">
         <v>404</v>
       </c>
       <c r="B46" s="32" t="s">
@@ -13057,7 +13735,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="110"/>
+      <c r="A47" s="113"/>
       <c r="B47" s="32" t="s">
         <v>407</v>
       </c>
@@ -13066,7 +13744,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="110"/>
+      <c r="A48" s="113"/>
       <c r="B48" s="32" t="s">
         <v>408</v>
       </c>
@@ -13075,7 +13753,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="110"/>
+      <c r="A49" s="113"/>
       <c r="B49" s="32" t="s">
         <v>410</v>
       </c>
@@ -13084,7 +13762,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="111"/>
+      <c r="A50" s="114"/>
       <c r="B50" s="32" t="s">
         <v>411</v>
       </c>
@@ -13101,7 +13779,7 @@
       <c r="B52" s="39"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="109" t="s">
+      <c r="A53" s="112" t="s">
         <v>412</v>
       </c>
       <c r="B53" s="32" t="s">
@@ -13112,7 +13790,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="110"/>
+      <c r="A54" s="113"/>
       <c r="B54" s="32" t="s">
         <v>414</v>
       </c>
@@ -13121,7 +13799,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="111"/>
+      <c r="A55" s="114"/>
       <c r="B55" s="32" t="s">
         <v>416</v>
       </c>
@@ -13635,7 +14313,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CAAF14-6D8F-425D-9DFC-A6859D0C7F1E}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:A14"/>
@@ -13691,17 +14369,17 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="144" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="119" t="s">
+      <c r="A8" s="122" t="s">
         <v>707</v>
       </c>
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="122"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -13709,25 +14387,19 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="127" t="s">
+      <c r="A11" s="123" t="s">
         <v>814</v>
       </c>
-      <c r="B11" s="125"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="128"/>
-      <c r="B12" s="125"/>
+      <c r="A12" s="124"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="128"/>
-      <c r="B13" s="125"/>
+      <c r="A13" s="124"/>
     </row>
     <row r="14" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="128"/>
-      <c r="B14" s="126"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="125"/>
+      <c r="A14" s="124"/>
+      <c r="B14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>